<commit_message>
a star time behalve cte matrix
</commit_message>
<xml_diff>
--- a/Instances/suitable_routes.xlsx
+++ b/Instances/suitable_routes.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25825"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="11_ED8330B498F18D8C9C69A35EBB4D514EC8CFCE3B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="11_ED8330B498F18D8C9C69A35EBB4D514EC8CFCE3B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1D8B4558-F245-4AD9-81FE-AE58705D9444}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" tabRatio="1000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14169" tabRatio="1000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Barge" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="12">
   <si>
     <t>O</t>
   </si>
@@ -63,7 +63,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -96,7 +96,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -374,15 +374,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B53"/>
+  <dimension ref="A1:B52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="F48" sqref="F48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -390,7 +393,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -398,7 +401,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -406,7 +409,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -414,7 +417,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -422,7 +425,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -430,7 +433,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -438,7 +441,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -446,7 +449,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -454,7 +457,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>2</v>
       </c>
@@ -462,7 +465,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -470,7 +473,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>2</v>
       </c>
@@ -478,7 +481,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -486,7 +489,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>3</v>
       </c>
@@ -494,7 +497,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>9</v>
       </c>
@@ -502,7 +505,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>3</v>
       </c>
@@ -510,7 +513,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>7</v>
       </c>
@@ -518,7 +521,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>3</v>
       </c>
@@ -526,7 +529,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>8</v>
       </c>
@@ -534,7 +537,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>5</v>
       </c>
@@ -542,7 +545,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>9</v>
       </c>
@@ -550,7 +553,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>5</v>
       </c>
@@ -558,7 +561,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>7</v>
       </c>
@@ -566,7 +569,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>5</v>
       </c>
@@ -574,7 +577,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>8</v>
       </c>
@@ -582,7 +585,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>10</v>
       </c>
@@ -590,7 +593,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>11</v>
       </c>
@@ -598,7 +601,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>10</v>
       </c>
@@ -606,7 +609,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>4</v>
       </c>
@@ -614,7 +617,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>10</v>
       </c>
@@ -622,7 +625,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>9</v>
       </c>
@@ -630,7 +633,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>10</v>
       </c>
@@ -638,7 +641,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>7</v>
       </c>
@@ -646,7 +649,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="34" spans="1:2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>10</v>
       </c>
@@ -654,7 +657,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>8</v>
       </c>
@@ -662,7 +665,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>11</v>
       </c>
@@ -670,7 +673,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>4</v>
       </c>
@@ -678,7 +681,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="38" spans="1:2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>11</v>
       </c>
@@ -686,7 +689,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="39" spans="1:2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>7</v>
       </c>
@@ -694,7 +697,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="40" spans="1:2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>11</v>
       </c>
@@ -702,7 +705,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="41" spans="1:2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>8</v>
       </c>
@@ -710,7 +713,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="42" spans="1:2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>4</v>
       </c>
@@ -718,7 +721,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="43" spans="1:2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>9</v>
       </c>
@@ -726,7 +729,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="44" spans="1:2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>4</v>
       </c>
@@ -734,7 +737,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="45" spans="1:2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>7</v>
       </c>
@@ -742,7 +745,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="46" spans="1:2">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>4</v>
       </c>
@@ -750,7 +753,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="47" spans="1:2">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>8</v>
       </c>
@@ -758,7 +761,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="48" spans="1:2">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>9</v>
       </c>
@@ -766,7 +769,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="49" spans="1:2">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>7</v>
       </c>
@@ -774,7 +777,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="50" spans="1:2">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>9</v>
       </c>
@@ -782,27 +785,19 @@
         <v>8</v>
       </c>
     </row>
-    <row r="51" spans="1:2">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B51" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B52" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2">
-      <c r="A53" t="s">
-        <v>8</v>
-      </c>
-      <c r="B53" t="s">
         <v>7</v>
       </c>
     </row>
@@ -816,12 +811,15 @@
   <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -829,7 +827,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -837,7 +835,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -845,7 +843,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -853,7 +851,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -861,7 +859,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -869,7 +867,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -877,7 +875,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -885,7 +883,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -893,7 +891,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -901,7 +899,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -909,7 +907,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>4</v>
       </c>
@@ -917,7 +915,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -925,7 +923,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>4</v>
       </c>
@@ -933,7 +931,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>7</v>
       </c>
@@ -941,7 +939,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>4</v>
       </c>
@@ -949,7 +947,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>8</v>
       </c>
@@ -957,7 +955,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>9</v>
       </c>
@@ -965,7 +963,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>7</v>
       </c>
@@ -973,7 +971,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>9</v>
       </c>
@@ -981,7 +979,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>8</v>
       </c>
@@ -989,7 +987,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>7</v>
       </c>
@@ -997,7 +995,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>8</v>
       </c>

</xml_diff>